<commit_message>
3 normalizacion y pdf de entrega con registros
</commit_message>
<xml_diff>
--- a/Modelo relacional.xlsx
+++ b/Modelo relacional.xlsx
@@ -8,12 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunez\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65C0936-5F06-420E-9BD6-AC54F8BBE772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3786D08B-B6D8-4CD1-B1BD-724A150DE2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FBD40ED5-9BFF-4BD4-A771-7F150652FE2B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Modelo Relacional" sheetId="1" r:id="rId1"/>
+    <sheet name="Atracciones" sheetId="2" r:id="rId2"/>
+    <sheet name="Operadores" sheetId="3" r:id="rId3"/>
+    <sheet name="Proveedores" sheetId="4" r:id="rId4"/>
+    <sheet name="Brazalete" sheetId="5" r:id="rId5"/>
+    <sheet name="Cliente" sheetId="6" r:id="rId6"/>
+    <sheet name="Orden de Servicio" sheetId="7" r:id="rId7"/>
+    <sheet name="Tecnicos" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,20 +32,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
   <si>
     <t>Atraccion</t>
   </si>
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
     <t>Fecha de adquisicion</t>
   </si>
   <si>
-    <t>Descripcion</t>
-  </si>
-  <si>
     <t>Proveedor</t>
   </si>
   <si>
@@ -145,13 +146,97 @@
   </si>
   <si>
     <t>Codigo Tecnicos</t>
+  </si>
+  <si>
+    <t>NombreOperador</t>
+  </si>
+  <si>
+    <t>NombreProveedor</t>
+  </si>
+  <si>
+    <t>NombreAtraccion</t>
+  </si>
+  <si>
+    <t>NombreCliente</t>
+  </si>
+  <si>
+    <t>NombreTecnico</t>
+  </si>
+  <si>
+    <t>DescripcionAtraccion</t>
+  </si>
+  <si>
+    <t>Montaña Extrema</t>
+  </si>
+  <si>
+    <t>20-15-2023</t>
+  </si>
+  <si>
+    <t>Montaña rusa de alta velocida</t>
+  </si>
+  <si>
+    <t>INT10</t>
+  </si>
+  <si>
+    <t>EXT</t>
+  </si>
+  <si>
+    <t>Roberto Gomez</t>
+  </si>
+  <si>
+    <t>15-3104692510</t>
+  </si>
+  <si>
+    <t>Mattel SAS</t>
+  </si>
+  <si>
+    <t>Rodeo Drive New York</t>
+  </si>
+  <si>
+    <t>customercare@mattel.com</t>
+  </si>
+  <si>
+    <t>Internacional</t>
+  </si>
+  <si>
+    <t>INT10 - 5655501</t>
+  </si>
+  <si>
+    <t>Extremo</t>
+  </si>
+  <si>
+    <t>Andres Vega</t>
+  </si>
+  <si>
+    <t>OS10</t>
+  </si>
+  <si>
+    <t>1 Dia</t>
+  </si>
+  <si>
+    <t>DescripcionServicio</t>
+  </si>
+  <si>
+    <t>Apretar ejes</t>
+  </si>
+  <si>
+    <t>TEC26</t>
+  </si>
+  <si>
+    <t>David Villa</t>
+  </si>
+  <si>
+    <t>Mecanica</t>
+  </si>
+  <si>
+    <t>TEC26 - 3226661025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,8 +252,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,8 +306,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -238,11 +345,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -257,10 +385,32 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1064,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216E7338-B6DA-4DAB-9AC1-83F4E1745135}">
-  <dimension ref="A2:K28"/>
+  <dimension ref="B2:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1081,219 +1231,215 @@
     <col min="11" max="11" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F3" s="5" t="s">
+      <c r="H5" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F5" s="2" t="s">
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F6" s="2" t="s">
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E11" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D12" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F10" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="E11" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D12" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="6" t="s">
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="10"/>
+      <c r="F17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D13" s="5" t="s">
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="H23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="F17" s="9" t="s">
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F20" t="s">
-        <v>25</v>
-      </c>
-      <c r="K20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F23" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F27" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F28" s="9" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1301,4 +1447,494 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514F3518-EB45-4CAA-B891-DE0F01293DC4}">
+  <dimension ref="B2:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770688CA-4732-4738-914F-5AB05BC3CC57}">
+  <dimension ref="B2:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="F2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D14" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F4:G4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F6B8678-5955-46DD-8ED7-CA0031A3242A}">
+  <dimension ref="B2:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="H2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H4:I4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{6BE928BB-F728-4A1F-A0AD-A2B82B17833B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14270F6E-AC9F-49C9-9046-1BF15CCD8914}">
+  <dimension ref="B2:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="20">
+        <v>44964</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DD8E1F-2A10-4DE8-B738-142AE8810F55}">
+  <dimension ref="B2:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>65656565</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="20">
+        <v>36022</v>
+      </c>
+      <c r="E4" s="2">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0D46B6-D5BB-444F-8F2D-0CF659DBB18F}">
+  <dimension ref="B2:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="20">
+        <v>44964</v>
+      </c>
+      <c r="D4" s="20">
+        <v>44965</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588308EE-7C94-43BB-A031-67EAFCA835D1}">
+  <dimension ref="B2:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="G2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>